<commit_message>
Dicionario de dados e modelagem logica
</commit_message>
<xml_diff>
--- a/banco de dados/dicionário_dados.xlsx
+++ b/banco de dados/dicionário_dados.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\GitHub\sdpiar\banco de dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E172A65-1E2C-45E7-BAF7-B72A69C2C604}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D6DE11-CAE1-4E5D-9F21-B991140B6690}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="90">
   <si>
     <t>Atributo</t>
   </si>
@@ -138,15 +138,9 @@
     <t>Tabela Usuário</t>
   </si>
   <si>
-    <t>Tabela área</t>
-  </si>
-  <si>
     <t>Identificação da área</t>
   </si>
   <si>
-    <t>Tabela TempArea</t>
-  </si>
-  <si>
     <t>Tabela Sensor</t>
   </si>
   <si>
@@ -157,9 +151,6 @@
   </si>
   <si>
     <t>Identificação do sensor</t>
-  </si>
-  <si>
-    <t>Irá identificar qual é a empresa que tem posse da área</t>
   </si>
   <si>
     <t>Irá identificar qual sensor está sendo medida a temperatura</t>
@@ -266,6 +257,45 @@
   </si>
   <si>
     <t>Empresa cadastrando funcionário</t>
+  </si>
+  <si>
+    <t>Tabela AreaBruto</t>
+  </si>
+  <si>
+    <t>Tabela area</t>
+  </si>
+  <si>
+    <t>Identificador do usuario</t>
+  </si>
+  <si>
+    <t>Chave Estrangeira</t>
+  </si>
+  <si>
+    <t>idsensor</t>
+  </si>
+  <si>
+    <t>fk_usuario</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>Irá identificar qual usuario é dono da area</t>
+  </si>
+  <si>
+    <t>Chave Primaria composta</t>
+  </si>
+  <si>
+    <t>fk_PRIMEIROSENSOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fk_SEGUNDOSENSOR </t>
+  </si>
+  <si>
+    <t>fk_TERCEIROSENSOR</t>
+  </si>
+  <si>
+    <t>fk_Area</t>
   </si>
 </sst>
 </file>
@@ -632,22 +662,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="63.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="63.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>36</v>
       </c>
@@ -657,7 +687,7 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -677,7 +707,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
@@ -685,25 +715,25 @@
         <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -711,7 +741,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
@@ -725,13 +755,13 @@
         <v>2</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>27</v>
       </c>
@@ -739,19 +769,19 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D6" s="1">
         <v>45</v>
       </c>
       <c r="E6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
@@ -759,19 +789,19 @@
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D7" s="1">
         <v>50</v>
       </c>
       <c r="E7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>29</v>
       </c>
@@ -779,19 +809,19 @@
         <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D8" s="1">
         <v>45</v>
       </c>
       <c r="E8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -799,7 +829,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D9" s="1">
         <v>15</v>
@@ -809,35 +839,35 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D10" s="1">
         <v>14</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D11" s="1">
         <v>45</v>
@@ -847,7 +877,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>31</v>
       </c>
@@ -855,19 +885,19 @@
         <v>12</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D12" s="1">
         <v>45</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>32</v>
       </c>
@@ -875,21 +905,21 @@
         <v>13</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D13" s="1">
         <v>45</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>37</v>
+        <v>78</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -897,7 +927,7 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>0</v>
       </c>
@@ -917,107 +947,103 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="1" t="s">
+      <c r="C20" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" s="1" t="s">
+      <c r="C21" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="E21" s="1" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>39</v>
+        <v>77</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1025,7 +1051,7 @@
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>0</v>
       </c>
@@ -1045,142 +1071,282 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D25" s="1">
         <v>5.2</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D26" s="1">
         <v>4.2</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D37" s="1">
+        <v>5.2</v>
+      </c>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
+      <c r="C38" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D38" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B39" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A30" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C32" s="1" t="s">
+      <c r="B40" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D32" s="1">
-        <v>5.2</v>
-      </c>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D33" s="1">
-        <v>3.1</v>
-      </c>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1" t="s">
-        <v>48</v>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1188,7 +1354,7 @@
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A15:F15"/>
     <mergeCell ref="A23:F23"/>
-    <mergeCell ref="A30:F30"/>
+    <mergeCell ref="A35:F35"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>